<commit_message>
Revised all graphs to fit new data
</commit_message>
<xml_diff>
--- a/aggregated_data_and_graphs.xlsx
+++ b/aggregated_data_and_graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9975"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Number Of Cores</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Total Simulation Runtime (in seconds)</t>
+  </si>
+  <si>
+    <t>Naïve Implementation</t>
   </si>
 </sst>
 </file>
@@ -88,6 +91,835 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Naïve Implementation - Sequential Average Travel Time</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5533</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="73836416"/>
+        <c:axId val="73837952"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="73836416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Cores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73837952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73837952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Travel Time (in seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73836416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Naïve Implementation - Sequential Total Simulation Runtime</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1303.1202000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="91820032"/>
+        <c:axId val="91821568"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="91820032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Cores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91821568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91821568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Simulation Time (in seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91820032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Naïve Implementation - Parallel Average Runtime</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5533.5625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5533.4375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5533.9140630000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5533.8789059999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6715.6416019999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="96368512"/>
+        <c:axId val="96370048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="96368512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Cores</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96370048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96370048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Runtime (in seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96368512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Naïve Implementation - Parallel Total Simulation Time</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>55.992400000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.778500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.849899999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.279600000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.2012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="96199808"/>
+        <c:axId val="96201344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="96199808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Cores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96201344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96201344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Simulation Runtime (in seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96199808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2162175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,10 +1238,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>648</v>
+        <v>5533</v>
       </c>
       <c r="C2" s="1">
-        <v>10.106400000000001</v>
+        <v>1303.1202000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -417,10 +1249,10 @@
         <v>64</v>
       </c>
       <c r="B3" s="1">
-        <v>644.0625</v>
+        <v>5533.5625</v>
       </c>
       <c r="C3" s="1">
-        <v>0.34129999999999999</v>
+        <v>55.992400000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -428,10 +1260,10 @@
         <v>128</v>
       </c>
       <c r="B4" s="1">
-        <v>645.1171875</v>
+        <v>5533.4375</v>
       </c>
       <c r="C4" s="1">
-        <v>0.18690000000000001</v>
+        <v>43.778500000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,10 +1271,10 @@
         <v>256</v>
       </c>
       <c r="B5" s="1">
-        <v>1471</v>
+        <v>5533.9140630000002</v>
       </c>
       <c r="C5" s="1">
-        <v>9.6699999999999994E-2</v>
+        <v>34.849899999999998</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,10 +1282,10 @@
         <v>512</v>
       </c>
       <c r="B6" s="1">
-        <v>537.234375</v>
+        <v>5533.8789059999999</v>
       </c>
       <c r="C6" s="1">
-        <v>0.126</v>
+        <v>36.279600000000002</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,15 +1293,21 @@
         <v>1024</v>
       </c>
       <c r="B7" s="1">
-        <v>380.83100000000002</v>
+        <v>6715.6416019999997</v>
       </c>
       <c r="C7" s="1">
-        <v>0.27489999999999998</v>
+        <v>18.2012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added 3 more columns to stats table
</commit_message>
<xml_diff>
--- a/aggregated_data_and_graphs.xlsx
+++ b/aggregated_data_and_graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="7680"/>
+    <workbookView xWindow="-15" yWindow="1215" windowWidth="24030" windowHeight="8910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Number Of Cores</t>
   </si>
@@ -28,6 +28,18 @@
   </si>
   <si>
     <t>Naïve Implementation</t>
+  </si>
+  <si>
+    <t>Autonomous Optimized Results</t>
+  </si>
+  <si>
+    <t>Event Rate (events / second)</t>
+  </si>
+  <si>
+    <t>Remote Sends</t>
+  </si>
+  <si>
+    <t>Remote Recvs</t>
   </si>
 </sst>
 </file>
@@ -71,13 +83,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -159,11 +178,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="73836416"/>
-        <c:axId val="73837952"/>
+        <c:axId val="41301504"/>
+        <c:axId val="41303424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73836416"/>
+        <c:axId val="41301504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -192,7 +211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73837952"/>
+        <c:crossAx val="41303424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -200,7 +219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73837952"/>
+        <c:axId val="41303424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,7 +254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73836416"/>
+        <c:crossAx val="41301504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -323,11 +342,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91820032"/>
-        <c:axId val="91821568"/>
+        <c:axId val="42147840"/>
+        <c:axId val="42149760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91820032"/>
+        <c:axId val="42147840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +375,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91821568"/>
+        <c:crossAx val="42149760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -364,7 +383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91821568"/>
+        <c:axId val="42149760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,7 +418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91820032"/>
+        <c:crossAx val="42147840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -511,11 +530,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96368512"/>
-        <c:axId val="96370048"/>
+        <c:axId val="42162432"/>
+        <c:axId val="42180992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96368512"/>
+        <c:axId val="42162432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +568,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96370048"/>
+        <c:crossAx val="42180992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -557,7 +576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96370048"/>
+        <c:axId val="42180992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96368512"/>
+        <c:crossAx val="42162432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -704,11 +723,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96199808"/>
-        <c:axId val="96201344"/>
+        <c:axId val="42205952"/>
+        <c:axId val="42207872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96199808"/>
+        <c:axId val="42205952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96201344"/>
+        <c:crossAx val="42207872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -745,7 +764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96201344"/>
+        <c:axId val="42207872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96199808"/>
+        <c:crossAx val="42205952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -801,16 +820,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -831,16 +850,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -861,16 +880,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -891,16 +910,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2162175</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1209,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,9 +1239,12 @@
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1232,8 +1254,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1243,8 +1274,17 @@
       <c r="C2" s="1">
         <v>1303.1202000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>228199.1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>64</v>
       </c>
@@ -1254,8 +1294,17 @@
       <c r="C3" s="1">
         <v>55.992400000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>5310919.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6200107</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6200107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>128</v>
       </c>
@@ -1265,8 +1314,17 @@
       <c r="C4" s="1">
         <v>43.778500000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>6792627.4000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6280776</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6280776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>256</v>
       </c>
@@ -1276,8 +1334,17 @@
       <c r="C5" s="1">
         <v>34.849899999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>8532909.4000000004</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6442406</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6442406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>512</v>
       </c>
@@ -1287,8 +1354,17 @@
       <c r="C6" s="1">
         <v>36.279600000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>8196640.9000000004</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6765830</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6765830</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1024</v>
       </c>
@@ -1298,8 +1374,17 @@
       <c r="C7" s="1">
         <v>18.2012</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>16347420.6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9828615</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9828615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1313,12 +1398,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4722</v>
+      </c>
+      <c r="C2" s="1">
+        <v>713.721</v>
+      </c>
+      <c r="D2" s="5">
+        <v>263315.09999999998</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4655.0625</v>
+      </c>
+      <c r="C3" s="1">
+        <v>67.389700000000005</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2772437.2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1300179</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1300179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4583.59375</v>
+      </c>
+      <c r="C4" s="1">
+        <v>34.467100000000002</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5371485.5999999996</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2612952</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2612952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3241.28125</v>
+      </c>
+      <c r="C5" s="1">
+        <v>18.5808</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9199654.4000000004</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2672039</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2672039</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>128</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>256</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>512</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>